<commit_message>
REFAC: merubah format export excel
</commit_message>
<xml_diff>
--- a/public/informasi_rak.xlsx
+++ b/public/informasi_rak.xlsx
@@ -26,40 +26,40 @@
     <t>Status Rak</t>
   </si>
   <si>
-    <t>Total Packing</t>
+    <t>Quantity</t>
   </si>
   <si>
     <t>Part Number</t>
   </si>
   <si>
+    <t>No Scan</t>
+  </si>
+  <si>
     <t>Tgl Checkin</t>
   </si>
   <si>
-    <t>A330</t>
-  </si>
-  <si>
-    <t>Kecil</t>
+    <t>B113</t>
+  </si>
+  <si>
+    <t>Besar</t>
   </si>
   <si>
     <t>Penuh</t>
   </si>
   <si>
-    <t>4111-03550-D</t>
-  </si>
-  <si>
-    <t>2023-12-06 14:20:19</t>
-  </si>
-  <si>
-    <t>B113</t>
-  </si>
-  <si>
-    <t>Besar</t>
-  </si>
-  <si>
     <t>4111-03550-C</t>
   </si>
   <si>
-    <t>2023-12-06 14:19:47</t>
+    <t>GQG9DB0W0T4XXP4Q</t>
+  </si>
+  <si>
+    <t>2023-12-08 15:53:51</t>
+  </si>
+  <si>
+    <t>GQG9DB0W0T4XXP4Q7</t>
+  </si>
+  <si>
+    <t>2023-12-11 07:12:19</t>
   </si>
   <si>
     <t>C001</t>
@@ -71,10 +71,10 @@
     <t>Terisi</t>
   </si>
   <si>
-    <t>4111-03550-C;4111-03550-D</t>
-  </si>
-  <si>
-    <t>2023-12-06 14:48:42</t>
+    <t>GQG9DB0W0T4XXP4Q8</t>
+  </si>
+  <si>
+    <t>2023-12-11 09:49:37</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,7 +422,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,48 +441,57 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -493,12 +502,15 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>